<commit_message>
updated backend and datasheet
</commit_message>
<xml_diff>
--- a/backend/datasheet.xlsx
+++ b/backend/datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="buffer"/>
@@ -15,60 +15,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>X</t>
   </si>
   <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Political Power</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Emissions</t>
+  </si>
+  <si>
+    <t>Resource Extraction (High Carbon)</t>
+  </si>
+  <si>
+    <t>Resource Extraction (Low Carbon)</t>
+  </si>
+  <si>
+    <t>Industrial (High Carbon)</t>
+  </si>
+  <si>
+    <t>Industrial (Low Carbon)</t>
+  </si>
+  <si>
+    <t>Consumer Goods (High Carbon)</t>
+  </si>
+  <si>
+    <t>Consumer Goods (Low Carbon)</t>
+  </si>
+  <si>
+    <t>Agriculture (High Carbon)</t>
+  </si>
+  <si>
+    <t>Agriculture (Low Carbon)</t>
+  </si>
+  <si>
+    <t>Energy (High Carbon)</t>
+  </si>
+  <si>
+    <t>Energy (Low Carbon)</t>
+  </si>
+  <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Political Power</t>
-  </si>
-  <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>Budget</t>
-  </si>
-  <si>
-    <t>Emissions</t>
-  </si>
-  <si>
-    <t>Resource Extraction (High Carbon)</t>
-  </si>
-  <si>
-    <t>Resource Extraction (Low Carbon)</t>
-  </si>
-  <si>
-    <t>Industrial (High Carbon)</t>
-  </si>
-  <si>
-    <t>Industrial (Low Carbon)</t>
-  </si>
-  <si>
-    <t>Consumer Goods (High Carbon)</t>
-  </si>
-  <si>
-    <t>Consumer Goods (Low Carbon)</t>
-  </si>
-  <si>
-    <t>Agriculture (High Carbon)</t>
-  </si>
-  <si>
-    <t>Agriculture (Low Carbon)</t>
-  </si>
-  <si>
-    <t>Energy (High Carbon)</t>
-  </si>
-  <si>
-    <t>Energy (Low Carbon)</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,18 +93,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -141,26 +132,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,18 +152,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -496,583 +460,583 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="B2" s="4">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="B3" s="4">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="B4" s="4">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="B5" s="4">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4">
+        <v>569</v>
+      </c>
+      <c r="D5" s="4">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>120</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="9">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="9">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="9">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="9">
-        <v>0</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="9">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9">
-        <v>0</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="9">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9">
-        <v>0</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="9">
-        <v>0</v>
-      </c>
-      <c r="C27" s="9">
-        <v>0</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="9">
-        <v>0</v>
-      </c>
-      <c r="C28" s="9">
-        <v>0</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="9">
-        <v>0</v>
-      </c>
-      <c r="C29" s="9">
-        <v>0</v>
-      </c>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="9">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9">
-        <v>0</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="9">
-        <v>0</v>
-      </c>
-      <c r="C32" s="9">
-        <v>0</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="9">
-        <v>0</v>
-      </c>
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
       <c r="A35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="9">
-        <v>0</v>
-      </c>
-      <c r="C35" s="9">
-        <v>0</v>
-      </c>
-      <c r="D35" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="9">
-        <v>0</v>
-      </c>
-      <c r="C36" s="9">
-        <v>0</v>
-      </c>
-      <c r="D36" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="9">
-        <v>0</v>
-      </c>
-      <c r="C37" s="9">
-        <v>0</v>
-      </c>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="9">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9">
-        <v>0</v>
-      </c>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="9">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9">
-        <v>0</v>
-      </c>
-      <c r="D40" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+      <c r="B40" s="4">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="9">
-        <v>0</v>
-      </c>
-      <c r="C41" s="9">
-        <v>0</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
       <c r="A43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="9">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+        <v>18</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="9">
-        <v>0</v>
-      </c>
-      <c r="C44" s="9">
-        <v>0</v>
-      </c>
-      <c r="D44" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="9">
-        <v>0</v>
-      </c>
-      <c r="C45" s="9">
-        <v>0</v>
-      </c>
-      <c r="D45" s="9">
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1088,17 +1052,17 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,63 +1076,63 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>569</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1176,8 +1140,8 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="4">
@@ -1190,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1204,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1226,8 +1190,8 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="4">
@@ -1240,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1276,8 +1240,8 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="4">
@@ -1318,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1327,7 +1291,7 @@
       <c r="D18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="4">
@@ -1368,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
@@ -1377,7 +1341,7 @@
       <c r="D22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="4">
@@ -1418,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1391,7 @@
       <c r="D26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="4">
@@ -1468,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
@@ -1477,7 +1441,7 @@
       <c r="D30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="4">
@@ -1504,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
@@ -1526,8 +1490,8 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+      <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="4">
@@ -1540,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -1554,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
@@ -1568,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -1576,8 +1540,8 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+      <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="4">
@@ -1590,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -1604,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
@@ -1618,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
@@ -1626,8 +1590,8 @@
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+      <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="4">
@@ -1640,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -1654,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
pushed changes to backend
</commit_message>
<xml_diff>
--- a/backend/datasheet.xlsx
+++ b/backend/datasheet.xlsx
@@ -4,18 +4,21 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="buffer"/>
     <sheet r:id="rId2" sheetId="2" name="Turn 1"/>
+    <sheet r:id="rId3" sheetId="3" name="Turn 2"/>
+    <sheet r:id="rId4" sheetId="4" name="Turn 3"/>
+    <sheet r:id="rId5" sheetId="5" name="Turn 4"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="18">
   <si>
     <t>X</t>
   </si>
@@ -70,22 +73,31 @@
   <si>
     <t>Energy (Low Carbon)</t>
   </si>
-  <si>
-    <t>USA</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -102,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -132,11 +144,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,13 +174,25 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -464,23 +503,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -488,77 +527,77 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4">
-        <v>35</v>
+      <c r="B2" s="10">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10">
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="10">
+        <v>45</v>
+      </c>
+      <c r="C3" s="10">
         <v>26</v>
       </c>
-      <c r="D3" s="4">
-        <v>48</v>
+      <c r="D3" s="10">
+        <v>234</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4">
-        <v>48</v>
-      </c>
-      <c r="D4" s="4">
-        <v>27</v>
+      <c r="B4" s="10">
+        <v>51</v>
+      </c>
+      <c r="C4" s="10">
+        <v>34</v>
+      </c>
+      <c r="D4" s="10">
+        <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4">
-        <v>569</v>
-      </c>
-      <c r="D5" s="4">
-        <v>59</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="B5" s="10">
+        <v>47</v>
+      </c>
+      <c r="C5" s="10">
+        <v>255</v>
+      </c>
+      <c r="D5" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
         <v>0</v>
       </c>
     </row>
@@ -566,13 +605,13 @@
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
         <v>0</v>
       </c>
     </row>
@@ -580,35 +619,35 @@
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
         <v>0</v>
       </c>
     </row>
@@ -616,13 +655,13 @@
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
         <v>0</v>
       </c>
     </row>
@@ -630,35 +669,35 @@
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
         <v>0</v>
       </c>
     </row>
@@ -666,13 +705,13 @@
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
         <v>0</v>
       </c>
     </row>
@@ -680,35 +719,35 @@
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
         <v>0</v>
       </c>
     </row>
@@ -716,13 +755,13 @@
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="4">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
         <v>0</v>
       </c>
     </row>
@@ -730,35 +769,35 @@
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="4">
-        <v>0</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
         <v>0</v>
       </c>
     </row>
@@ -766,13 +805,13 @@
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="4">
-        <v>0</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
         <v>0</v>
       </c>
     </row>
@@ -780,35 +819,35 @@
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="4">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="4">
-        <v>0</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0</v>
-      </c>
-      <c r="D27" s="4">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
         <v>0</v>
       </c>
     </row>
@@ -816,13 +855,13 @@
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="4">
-        <v>0</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4">
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
         <v>0</v>
       </c>
     </row>
@@ -830,35 +869,35 @@
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="4">
-        <v>0</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
         <v>0</v>
       </c>
     </row>
@@ -866,13 +905,13 @@
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="4">
-        <v>0</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4">
+      <c r="B32" s="10">
+        <v>0</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
         <v>0</v>
       </c>
     </row>
@@ -880,13 +919,13 @@
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="4">
-        <v>0</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0</v>
-      </c>
-      <c r="D33" s="4">
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
         <v>0</v>
       </c>
     </row>
@@ -894,21 +933,21 @@
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
-      <c r="A35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="4">
-        <v>0</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4">
+      <c r="A35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
         <v>0</v>
       </c>
     </row>
@@ -916,13 +955,13 @@
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="4">
-        <v>0</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4">
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
         <v>0</v>
       </c>
     </row>
@@ -930,13 +969,13 @@
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="4">
-        <v>0</v>
-      </c>
-      <c r="C37" s="4">
-        <v>0</v>
-      </c>
-      <c r="D37" s="4">
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
         <v>0</v>
       </c>
     </row>
@@ -944,21 +983,21 @@
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
-      <c r="A39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="4">
-        <v>0</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0</v>
-      </c>
-      <c r="D39" s="4">
+      <c r="A39" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
         <v>0</v>
       </c>
     </row>
@@ -966,13 +1005,13 @@
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="4">
-        <v>0</v>
-      </c>
-      <c r="C40" s="4">
-        <v>0</v>
-      </c>
-      <c r="D40" s="4">
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
         <v>0</v>
       </c>
     </row>
@@ -980,13 +1019,13 @@
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="4">
-        <v>0</v>
-      </c>
-      <c r="C41" s="4">
-        <v>0</v>
-      </c>
-      <c r="D41" s="4">
+      <c r="B41" s="10">
+        <v>0</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
         <v>0</v>
       </c>
     </row>
@@ -994,21 +1033,21 @@
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
-      <c r="A43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="4">
-        <v>0</v>
-      </c>
-      <c r="C43" s="4">
-        <v>0</v>
-      </c>
-      <c r="D43" s="4">
+      <c r="A43" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1016,13 +1055,13 @@
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="4">
-        <v>0</v>
-      </c>
-      <c r="C44" s="4">
-        <v>0</v>
-      </c>
-      <c r="D44" s="4">
+      <c r="B44" s="10">
+        <v>0</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1030,13 +1069,13 @@
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="4">
-        <v>0</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0</v>
-      </c>
-      <c r="D45" s="4">
+      <c r="B45" s="10">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1052,17 +1091,1793 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="22.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10">
+        <v>24</v>
+      </c>
+      <c r="D2" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10">
+        <v>26</v>
+      </c>
+      <c r="D3" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10">
+        <v>48</v>
+      </c>
+      <c r="D4" s="10">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" s="10">
+        <v>569</v>
+      </c>
+      <c r="D5" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="A26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+      <c r="A34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+      <c r="A35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+      <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+      <c r="A39" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
+      <c r="A40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
+      <c r="A41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
+      <c r="A42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+      <c r="A43" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+      <c r="A44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="10">
+        <v>0</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
+      <c r="A45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="10">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10">
+        <v>45</v>
+      </c>
+      <c r="C3" s="10">
+        <v>26</v>
+      </c>
+      <c r="D3" s="10">
+        <v>234</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10">
+        <v>51</v>
+      </c>
+      <c r="C4" s="10">
+        <v>34</v>
+      </c>
+      <c r="D4" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="10">
+        <v>47</v>
+      </c>
+      <c r="C5" s="10">
+        <v>255</v>
+      </c>
+      <c r="D5" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+      <c r="A26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
+      <c r="A32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+      <c r="A34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+      <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
+      <c r="A40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
+      <c r="A41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
+      <c r="A42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+      <c r="A44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="10">
+        <v>0</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
+      <c r="A45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="10">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10">
+        <v>35</v>
+      </c>
+      <c r="D2" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10">
+        <v>26</v>
+      </c>
+      <c r="C3" s="10">
+        <v>47</v>
+      </c>
+      <c r="D3" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10">
+        <v>35</v>
+      </c>
+      <c r="C4" s="10">
+        <v>26</v>
+      </c>
+      <c r="D4" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="10">
+        <v>58</v>
+      </c>
+      <c r="C5" s="10">
+        <v>345</v>
+      </c>
+      <c r="D5" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+      <c r="A26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="A32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+      <c r="A34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+      <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
+      <c r="A40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
+      <c r="A41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
+      <c r="A42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+      <c r="A44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="10">
+        <v>0</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
+      <c r="A45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="10">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D45"/>
+  <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1076,72 +2891,72 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
-        <v>12</v>
+        <v>734</v>
       </c>
       <c r="C2" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4">
-        <v>48</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+        <v>234</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4">
+        <v>588</v>
+      </c>
+      <c r="D5" s="4">
         <v>25</v>
       </c>
-      <c r="C5" s="4">
-        <v>569</v>
-      </c>
-      <c r="D5" s="4">
-        <v>59</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="4">
@@ -1154,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1168,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1182,16 +2997,16 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="4">
@@ -1204,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1218,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -1232,16 +3047,16 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+      <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="4">
@@ -1254,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1268,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -1282,16 +3097,16 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+      <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="4">
@@ -1304,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1318,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
@@ -1332,16 +3147,16 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+      <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="4">
@@ -1354,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -1368,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -1382,16 +3197,16 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="2" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+      <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="4">
@@ -1404,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1418,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -1432,16 +3247,16 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="2" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+      <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="4">
@@ -1454,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
@@ -1486,12 +3301,12 @@
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="4">
@@ -1536,12 +3351,12 @@
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="4">
@@ -1586,12 +3401,12 @@
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="4">

</xml_diff>